<commit_message>
wip for new file path code
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GregoryT\Source\Repos\OpenInApp.Launcher\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="15150" windowHeight="9540"/>
   </bookViews>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="89">
   <si>
     <t>C:\Program Files\Firefox Developer Edition\firefox.exe</t>
   </si>
@@ -466,6 +471,9 @@
   </si>
   <si>
     <t>AlternativeTopLevelFolderType</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -557,6 +565,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -604,7 +615,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -639,7 +650,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -848,10 +859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F135"/>
+  <dimension ref="A1:G135"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -861,10 +872,12 @@
     <col min="3" max="3" width="21.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="57.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.33203125" style="4"/>
+    <col min="6" max="8" width="9.33203125" style="4"/>
+    <col min="9" max="9" width="57.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.33203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>86</v>
       </c>
@@ -881,7 +894,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -901,7 +914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -920,8 +933,11 @@
       <c r="F3" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -940,8 +956,11 @@
       <c r="F4" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -960,8 +979,11 @@
       <c r="F5" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -980,8 +1002,11 @@
       <c r="F6" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -1000,8 +1025,11 @@
       <c r="F7" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -1020,8 +1048,11 @@
       <c r="F8" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
@@ -1040,8 +1071,11 @@
       <c r="F9" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -1060,8 +1094,11 @@
       <c r="F10" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
@@ -1080,8 +1117,11 @@
       <c r="F11" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1100,8 +1140,11 @@
       <c r="F12" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
@@ -1120,8 +1163,11 @@
       <c r="F13" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>0</v>
       </c>
@@ -1140,8 +1186,11 @@
       <c r="F14" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
@@ -1160,8 +1209,11 @@
       <c r="F15" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>1</v>
       </c>
@@ -1180,8 +1232,11 @@
       <c r="F16" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>9</v>
       </c>
@@ -1200,8 +1255,11 @@
       <c r="F17" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>10</v>
       </c>
@@ -1221,7 +1279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>11</v>
       </c>
@@ -1240,8 +1298,11 @@
       <c r="F19" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
wip refactorings (not compiling)
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="88">
   <si>
     <t>C:\Program Files\Firefox Developer Edition\firefox.exe</t>
   </si>
@@ -471,9 +471,6 @@
   </si>
   <si>
     <t>AlternativeTopLevelFolderType</t>
-  </si>
-  <si>
-    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -518,12 +515,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -538,7 +541,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -553,6 +556,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -859,25 +865,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G135"/>
+  <dimension ref="A1:F135"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="78.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="4" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="57.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9.33203125" style="4"/>
+    <col min="6" max="6" width="13" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.33203125" style="4"/>
     <col min="9" max="9" width="57.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.33203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>86</v>
       </c>
@@ -894,7 +901,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -910,11 +917,11 @@
       <c r="E2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="4" t="b">
+      <c r="F2" s="6" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -933,11 +940,8 @@
       <c r="F3" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -956,11 +960,8 @@
       <c r="F4" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -979,11 +980,8 @@
       <c r="F5" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -1002,11 +1000,8 @@
       <c r="F6" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -1025,11 +1020,8 @@
       <c r="F7" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -1048,11 +1040,8 @@
       <c r="F8" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
@@ -1071,11 +1060,8 @@
       <c r="F9" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -1094,11 +1080,8 @@
       <c r="F10" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
@@ -1117,11 +1100,8 @@
       <c r="F11" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1140,11 +1120,8 @@
       <c r="F12" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
@@ -1163,11 +1140,8 @@
       <c r="F13" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>0</v>
       </c>
@@ -1186,11 +1160,8 @@
       <c r="F14" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
@@ -1209,11 +1180,8 @@
       <c r="F15" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>1</v>
       </c>
@@ -1232,11 +1200,8 @@
       <c r="F16" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>9</v>
       </c>
@@ -1255,21 +1220,18 @@
       <c r="F17" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="G17" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="6" t="s">
         <v>82</v>
       </c>
       <c r="E18" s="3" t="s">
@@ -1279,7 +1241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>11</v>
       </c>
@@ -1298,11 +1260,8 @@
       <c r="F19" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="G19" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
continuance of wip (now compiling)
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GregoryT\Source\Repos\OpenInApp.Launcher\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="15150" windowHeight="9540"/>
   </bookViews>
@@ -515,7 +510,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -525,6 +520,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -541,7 +542,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -559,6 +560,18 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -621,7 +634,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -656,7 +669,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -868,7 +881,7 @@
   <dimension ref="A1:F135"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -905,16 +918,16 @@
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="9" t="s">
         <v>52</v>
       </c>
       <c r="F2" s="6" t="b">
@@ -925,19 +938,19 @@
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="4" t="b">
+      <c r="F3" s="7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -945,19 +958,19 @@
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="4" t="b">
+      <c r="F4" s="7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -965,19 +978,19 @@
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="4" t="b">
+      <c r="F5" s="7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -985,19 +998,19 @@
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="4" t="b">
+      <c r="F6" s="7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1005,19 +1018,19 @@
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F7" s="4" t="b">
+      <c r="F7" s="7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1025,19 +1038,19 @@
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F8" s="4" t="b">
+      <c r="F8" s="7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1045,19 +1058,19 @@
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F9" s="4" t="b">
+      <c r="F9" s="7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1065,19 +1078,19 @@
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="4" t="b">
+      <c r="F10" s="7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1085,19 +1098,19 @@
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="4" t="b">
+      <c r="F11" s="7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1105,19 +1118,19 @@
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="4" t="b">
+      <c r="F12" s="7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1125,19 +1138,19 @@
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="4" t="b">
+      <c r="F13" s="7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1145,19 +1158,19 @@
       <c r="A14" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="4" t="b">
+      <c r="F14" s="7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1165,19 +1178,19 @@
       <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="4" t="b">
+      <c r="F15" s="7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1185,19 +1198,19 @@
       <c r="A16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="F16" s="4" t="b">
+      <c r="F16" s="7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1205,19 +1218,19 @@
       <c r="A17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="4" t="b">
+      <c r="F17" s="7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1234,10 +1247,10 @@
       <c r="D18" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="4" t="b">
+      <c r="F18" s="7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1245,19 +1258,19 @@
       <c r="A19" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="F19" s="4" t="b">
+      <c r="F19" s="7" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
more code centralisation for easier testing
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GregoryT\Source\Repos\OpenInApp.Launcher\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="15150" windowHeight="9540"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="15150" windowHeight="9540" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="109">
   <si>
     <t>C:\Program Files\Firefox Developer Edition\firefox.exe</t>
   </si>
@@ -467,12 +473,106 @@
   <si>
     <t>AlternativeTopLevelFolderType</t>
   </si>
+  <si>
+    <t>[TestCase("</t>
+  </si>
+  <si>
+    <r>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)]</t>
+    </r>
+  </si>
+  <si>
+    <t>[TestCase("XMLSpy.exe", "C:\Program Files (x86)\Altova\XMLSpy2016\XMLSpy.exe")]</t>
+  </si>
+  <si>
+    <t>[TestCase("gimp-2.8.exe", "C:\Program Files (x86)\bin\gimp-2.8.exe")]</t>
+  </si>
+  <si>
+    <t>[TestCase("MarkdownMonster.exe", "C:\Program Files (x86)\Markdown Monster\MarkdownMonster.exe")]</t>
+  </si>
+  <si>
+    <t>[TestCase("devenv.exe", "C:\Program Files (x86)\Microsoft Visual Studio 11.0\Common7\IDE\devenv.exe")]</t>
+  </si>
+  <si>
+    <t>[TestCase("devenv.exe", "C:\Program Files (x86)\Microsoft Visual Studio 12.0\Common7\IDE\devenv.exe")]</t>
+  </si>
+  <si>
+    <t>[TestCase("devenv.exe", "C:\Program Files (x86)\Microsoft Visual Studio 14.0\Common7\IDE\devenv.exe")]</t>
+  </si>
+  <si>
+    <t>[TestCase("devenv.exe", "C:\Program Files (x86)\Microsoft Visual Studio\2017\Community\Common7\IDE\devenv.exe")]</t>
+  </si>
+  <si>
+    <t>[TestCase("devenv.exe", "C:\Program Files (x86)\Microsoft Visual Studio\2017\Enterprise\Common7\IDE\devenv.exe")]</t>
+  </si>
+  <si>
+    <t>[TestCase("devenv.exe", "C:\Program Files (x86)\Microsoft Visual Studio\2017\Professional\Common7\IDE\devenv.exe")]</t>
+  </si>
+  <si>
+    <t>[TestCase("opera.exe", "C:\Program Files (x86)\Opera\opera.exe")]</t>
+  </si>
+  <si>
+    <t>[TestCase("PaintDotNet.exe", "C:\Program Files (x86)\Paint.NET\PaintDotNet.exe")]</t>
+  </si>
+  <si>
+    <t>[TestCase("XamarinStudio.exe", "C:\Program Files (x86)\Xamarin Studio\bin\XamarinStudio.exe")]</t>
+  </si>
+  <si>
+    <t>[TestCase("firefox.exe", "C:\Program Files\Firefox Developer Edition\firefox.exe")]</t>
+  </si>
+  <si>
+    <t>[TestCase("launcher.exe", "C:\Program Files\Opera developer\launcher.exe")]</t>
+  </si>
+  <si>
+    <t>[TestCase("chrome.exe", "C:\Users\greg\AppData\Local\Google\Chrome SxS\Application\chrome.exe")]</t>
+  </si>
+  <si>
+    <t>[TestCase("vivaldi.exe", "C:\Users\greg\AppData\Local\Vivaldi\Application\vivaldi.exe")]</t>
+  </si>
+  <si>
+    <t>[TestCase("runemacs.exe", "C:\Users\greg\Desktop\ZZZ open in\_emacs-25.1-2-x86_64-w64-mingw32\bin\runemacs.exe")]</t>
+  </si>
+  <si>
+    <t>[TestCase("mspaint.exe ", "C:\Windows\system32\mspaint.exe ")]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <color theme="1"/>
@@ -509,6 +609,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFA31515"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -542,7 +648,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -573,6 +679,21 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -634,7 +755,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -669,7 +790,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -880,8 +1001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1756,4 +1877,576 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I133"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="13" customWidth="1"/>
+    <col min="4" max="4" width="83.5" style="13" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" style="13"/>
+    <col min="6" max="6" width="57.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.33203125" style="13"/>
+    <col min="9" max="9" width="49.6640625" style="13" customWidth="1"/>
+    <col min="10" max="16384" width="9.33203125" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="11" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="B1" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="101.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="13" t="str">
+        <f>CONCATENATE(A2,B2,C2,D2,E2)</f>
+        <v>[TestCase("XMLSpy.exe", "C:\Program Files (x86)\Altova\XMLSpy2016\XMLSpy.exe")]</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="90" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="13" t="str">
+        <f t="shared" ref="F3:F19" si="0">CONCATENATE(A3,B3,C3,D3,E3)</f>
+        <v>[TestCase("gimp-2.8.exe", "C:\Program Files (x86)\bin\gimp-2.8.exe")]</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="135" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>[TestCase("MarkdownMonster.exe", "C:\Program Files (x86)\Markdown Monster\MarkdownMonster.exe")]</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="123.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>[TestCase("devenv.exe", "C:\Program Files (x86)\Microsoft Visual Studio 11.0\Common7\IDE\devenv.exe")]</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="123.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>[TestCase("devenv.exe", "C:\Program Files (x86)\Microsoft Visual Studio 12.0\Common7\IDE\devenv.exe")]</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="123.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>[TestCase("devenv.exe", "C:\Program Files (x86)\Microsoft Visual Studio 14.0\Common7\IDE\devenv.exe")]</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="146.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>[TestCase("devenv.exe", "C:\Program Files (x86)\Microsoft Visual Studio\2017\Community\Common7\IDE\devenv.exe")]</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="146.25" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>[TestCase("devenv.exe", "C:\Program Files (x86)\Microsoft Visual Studio\2017\Enterprise\Common7\IDE\devenv.exe")]</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="146.25" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>[TestCase("devenv.exe", "C:\Program Files (x86)\Microsoft Visual Studio\2017\Professional\Common7\IDE\devenv.exe")]</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="78.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>[TestCase("opera.exe", "C:\Program Files (x86)\Opera\opera.exe")]</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="101.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>[TestCase("PaintDotNet.exe", "C:\Program Files (x86)\Paint.NET\PaintDotNet.exe")]</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="112.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F13" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>[TestCase("XamarinStudio.exe", "C:\Program Files (x86)\Xamarin Studio\bin\XamarinStudio.exe")]</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="101.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>[TestCase("firefox.exe", "C:\Program Files\Firefox Developer Edition\firefox.exe")]</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="90" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F15" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>[TestCase("launcher.exe", "C:\Program Files\Opera developer\launcher.exe")]</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="123.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>[TestCase("chrome.exe", "C:\Users\greg\AppData\Local\Google\Chrome SxS\Application\chrome.exe")]</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="101.25" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F17" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>[TestCase("vivaldi.exe", "C:\Users\greg\AppData\Local\Vivaldi\Application\vivaldi.exe")]</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="168.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F18" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>[TestCase("runemacs.exe", "C:\Users\greg\Desktop\ZZZ open in\_emacs-25.1-2-x86_64-w64-mingw32\bin\runemacs.exe")]</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="78.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>[TestCase("mspaint.exe ", "C:\Windows\system32\mspaint.exe ")]</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" s="12"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" s="12"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" s="12"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" s="12"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" s="12"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" s="12"/>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104" s="12"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105" s="12"/>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106" s="12"/>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" s="12"/>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108" s="12"/>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109" s="12"/>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110" s="12"/>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111" s="12"/>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112" s="12"/>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113" s="12"/>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114" s="12"/>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115" s="12"/>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116" s="12"/>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117" s="12"/>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118" s="12"/>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119" s="12"/>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120" s="12"/>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121" s="12"/>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122" s="12"/>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A123" s="12"/>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A124" s="12"/>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A125" s="12"/>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A126" s="12"/>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A127" s="12"/>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A128" s="12"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A129" s="12"/>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A130" s="12"/>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131" s="12"/>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132" s="12"/>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>